<commit_message>
daily auto push: 2025-08-11 07:02 UTC
</commit_message>
<xml_diff>
--- a/excel/apple3.xlsx
+++ b/excel/apple3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2030"/>
+  <dimension ref="A1:D2031"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -36977,6 +36977,24 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2031">
+      <c r="A2031" t="inlineStr">
+        <is>
+          <t>2025/08/11</t>
+        </is>
+      </c>
+      <c r="B2031" t="inlineStr">
+        <is>
+          <t>月</t>
+        </is>
+      </c>
+      <c r="C2031" t="n">
+        <v>14</v>
+      </c>
+      <c r="D2031" t="n">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
daily auto push: 2025-09-11 03:06 UTC
</commit_message>
<xml_diff>
--- a/excel/apple3.xlsx
+++ b/excel/apple3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2230"/>
+  <dimension ref="A1:D2231"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -40577,6 +40577,24 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2231">
+      <c r="A2231" t="inlineStr">
+        <is>
+          <t>2025/09/11</t>
+        </is>
+      </c>
+      <c r="B2231" t="inlineStr">
+        <is>
+          <t>木</t>
+        </is>
+      </c>
+      <c r="C2231" t="n">
+        <v>11</v>
+      </c>
+      <c r="D2231" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
daily auto push: 2025-12-10 07:33 UTC
</commit_message>
<xml_diff>
--- a/excel/apple3.xlsx
+++ b/excel/apple3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2668"/>
+  <dimension ref="A1:D2669"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -48461,6 +48461,24 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2669">
+      <c r="A2669" t="inlineStr">
+        <is>
+          <t>2025/12/10</t>
+        </is>
+      </c>
+      <c r="B2669" t="inlineStr">
+        <is>
+          <t>水</t>
+        </is>
+      </c>
+      <c r="C2669" t="n">
+        <v>15</v>
+      </c>
+      <c r="D2669" t="n">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
daily auto push: 2026-02-23 10:07 UTC
</commit_message>
<xml_diff>
--- a/excel/apple3.xlsx
+++ b/excel/apple3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3162"/>
+  <dimension ref="A1:D3163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -56600,19 +56600,19 @@
     <row r="3121">
       <c r="A3121" t="inlineStr">
         <is>
-          <t>2026/12/29</t>
+          <t>2026/02/23</t>
         </is>
       </c>
       <c r="B3121" t="inlineStr">
         <is>
-          <t>火</t>
+          <t>月</t>
         </is>
       </c>
       <c r="C3121" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D3121" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3122">
@@ -56627,7 +56627,7 @@
         </is>
       </c>
       <c r="C3122" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3122" t="n">
         <v>3</v>
@@ -56645,7 +56645,7 @@
         </is>
       </c>
       <c r="C3123" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3123" t="n">
         <v>3</v>
@@ -56663,7 +56663,7 @@
         </is>
       </c>
       <c r="C3124" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D3124" t="n">
         <v>3</v>
@@ -56672,16 +56672,16 @@
     <row r="3125">
       <c r="A3125" t="inlineStr">
         <is>
-          <t>2026/12/30</t>
+          <t>2026/12/29</t>
         </is>
       </c>
       <c r="B3125" t="inlineStr">
         <is>
-          <t>水</t>
+          <t>火</t>
         </is>
       </c>
       <c r="C3125" t="n">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D3125" t="n">
         <v>3</v>
@@ -56699,7 +56699,7 @@
         </is>
       </c>
       <c r="C3126" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D3126" t="n">
         <v>3</v>
@@ -56717,7 +56717,7 @@
         </is>
       </c>
       <c r="C3127" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3127" t="n">
         <v>3</v>
@@ -56735,7 +56735,7 @@
         </is>
       </c>
       <c r="C3128" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D3128" t="n">
         <v>3</v>
@@ -56753,7 +56753,7 @@
         </is>
       </c>
       <c r="C3129" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3129" t="n">
         <v>3</v>
@@ -56771,7 +56771,7 @@
         </is>
       </c>
       <c r="C3130" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D3130" t="n">
         <v>3</v>
@@ -56780,16 +56780,16 @@
     <row r="3131">
       <c r="A3131" t="inlineStr">
         <is>
-          <t>2026/12/31</t>
+          <t>2026/12/30</t>
         </is>
       </c>
       <c r="B3131" t="inlineStr">
         <is>
-          <t>木</t>
+          <t>水</t>
         </is>
       </c>
       <c r="C3131" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D3131" t="n">
         <v>3</v>
@@ -56807,7 +56807,7 @@
         </is>
       </c>
       <c r="C3132" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D3132" t="n">
         <v>3</v>
@@ -56825,7 +56825,7 @@
         </is>
       </c>
       <c r="C3133" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3133" t="n">
         <v>3</v>
@@ -56843,7 +56843,7 @@
         </is>
       </c>
       <c r="C3134" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D3134" t="n">
         <v>3</v>
@@ -56861,7 +56861,7 @@
         </is>
       </c>
       <c r="C3135" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3135" t="n">
         <v>3</v>
@@ -56879,7 +56879,7 @@
         </is>
       </c>
       <c r="C3136" t="n">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D3136" t="n">
         <v>3</v>
@@ -56888,16 +56888,16 @@
     <row r="3137">
       <c r="A3137" t="inlineStr">
         <is>
-          <t>2027/01/01</t>
+          <t>2026/12/31</t>
         </is>
       </c>
       <c r="B3137" t="inlineStr">
         <is>
-          <t>金</t>
+          <t>木</t>
         </is>
       </c>
       <c r="C3137" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D3137" t="n">
         <v>3</v>
@@ -56915,7 +56915,7 @@
         </is>
       </c>
       <c r="C3138" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D3138" t="n">
         <v>3</v>
@@ -56933,7 +56933,7 @@
         </is>
       </c>
       <c r="C3139" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D3139" t="n">
         <v>3</v>
@@ -56951,7 +56951,7 @@
         </is>
       </c>
       <c r="C3140" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3140" t="n">
         <v>3</v>
@@ -56969,7 +56969,7 @@
         </is>
       </c>
       <c r="C3141" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3141" t="n">
         <v>3</v>
@@ -56978,16 +56978,16 @@
     <row r="3142">
       <c r="A3142" t="inlineStr">
         <is>
-          <t>2027/01/02</t>
+          <t>2027/01/01</t>
         </is>
       </c>
       <c r="B3142" t="inlineStr">
         <is>
-          <t>土</t>
+          <t>金</t>
         </is>
       </c>
       <c r="C3142" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D3142" t="n">
         <v>3</v>
@@ -57005,7 +57005,7 @@
         </is>
       </c>
       <c r="C3143" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D3143" t="n">
         <v>3</v>
@@ -57023,7 +57023,7 @@
         </is>
       </c>
       <c r="C3144" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3144" t="n">
         <v>3</v>
@@ -57041,10 +57041,10 @@
         </is>
       </c>
       <c r="C3145" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D3145" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3146">
@@ -57059,7 +57059,7 @@
         </is>
       </c>
       <c r="C3146" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3146" t="n">
         <v>2</v>
@@ -57077,7 +57077,7 @@
         </is>
       </c>
       <c r="C3147" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3147" t="n">
         <v>2</v>
@@ -57095,7 +57095,7 @@
         </is>
       </c>
       <c r="C3148" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3148" t="n">
         <v>2</v>
@@ -57104,16 +57104,16 @@
     <row r="3149">
       <c r="A3149" t="inlineStr">
         <is>
-          <t>2027/01/03</t>
+          <t>2027/01/02</t>
         </is>
       </c>
       <c r="B3149" t="inlineStr">
         <is>
-          <t>日</t>
+          <t>土</t>
         </is>
       </c>
       <c r="C3149" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="D3149" t="n">
         <v>2</v>
@@ -57131,10 +57131,10 @@
         </is>
       </c>
       <c r="C3150" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D3150" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3151">
@@ -57149,7 +57149,7 @@
         </is>
       </c>
       <c r="C3151" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D3151" t="n">
         <v>3</v>
@@ -57167,7 +57167,7 @@
         </is>
       </c>
       <c r="C3152" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D3152" t="n">
         <v>3</v>
@@ -57185,7 +57185,7 @@
         </is>
       </c>
       <c r="C3153" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3153" t="n">
         <v>3</v>
@@ -57203,7 +57203,7 @@
         </is>
       </c>
       <c r="C3154" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3154" t="n">
         <v>3</v>
@@ -57221,7 +57221,7 @@
         </is>
       </c>
       <c r="C3155" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3155" t="n">
         <v>3</v>
@@ -57230,16 +57230,16 @@
     <row r="3156">
       <c r="A3156" t="inlineStr">
         <is>
-          <t>2027/01/04</t>
+          <t>2027/01/03</t>
         </is>
       </c>
       <c r="B3156" t="inlineStr">
         <is>
-          <t>月</t>
+          <t>日</t>
         </is>
       </c>
       <c r="C3156" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D3156" t="n">
         <v>3</v>
@@ -57257,10 +57257,10 @@
         </is>
       </c>
       <c r="C3157" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D3157" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3158">
@@ -57275,7 +57275,7 @@
         </is>
       </c>
       <c r="C3158" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D3158" t="n">
         <v>4</v>
@@ -57293,10 +57293,10 @@
         </is>
       </c>
       <c r="C3159" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D3159" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3160">
@@ -57311,7 +57311,7 @@
         </is>
       </c>
       <c r="C3160" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D3160" t="n">
         <v>3</v>
@@ -57320,16 +57320,16 @@
     <row r="3161">
       <c r="A3161" t="inlineStr">
         <is>
-          <t>2027/01/05</t>
+          <t>2027/01/04</t>
         </is>
       </c>
       <c r="B3161" t="inlineStr">
         <is>
-          <t>火</t>
+          <t>月</t>
         </is>
       </c>
       <c r="C3161" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="D3161" t="n">
         <v>3</v>
@@ -57347,9 +57347,27 @@
         </is>
       </c>
       <c r="C3162" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3162" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3163">
+      <c r="A3163" t="inlineStr">
+        <is>
+          <t>2027/01/05</t>
+        </is>
+      </c>
+      <c r="B3163" t="inlineStr">
+        <is>
+          <t>火</t>
+        </is>
+      </c>
+      <c r="C3163" t="n">
         <v>7</v>
       </c>
-      <c r="D3162" t="n">
+      <c r="D3163" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>